<commit_message>
position and cash output OK
</commit_message>
<xml_diff>
--- a/samples/Cash Stt _04112019.xlsx
+++ b/samples/Cash Stt _04112019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Reconciliation\In-house Fund\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\bochk_revised\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42C8561E-9C18-42E4-9864-B8823C1A7381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235C5E5B-3A3D-4CD0-B758-732295B77490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30480" yWindow="4365" windowWidth="24525" windowHeight="12225"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accttxdtl_001 - 2019-11-05T0952" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -977,11 +977,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,10 +1278,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>